<commit_message>
Tuesday4Feb25 time formatted good
</commit_message>
<xml_diff>
--- a/public/excel/711.xlsx
+++ b/public/excel/711.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NeilCumming\Atm-Bus\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NeilCumming\Atm-Bus\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE361CBC-06DA-4773-A949-B9F6308FD077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80299297-260B-416F-813E-67F8D268A2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30420" yWindow="990" windowWidth="12645" windowHeight="13485" xr2:uid="{CB2D3FB0-89E8-4325-887F-CAFE9D99A230}"/>
+    <workbookView xWindow="384" yWindow="2220" windowWidth="15912" windowHeight="10740" xr2:uid="{CB2D3FB0-89E8-4325-887F-CAFE9D99A230}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -215,7 +215,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AB1D25-2BFA-4B40-89BF-7C3A7093603D}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,7 +593,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -607,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.37638888888888888</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -621,7 +621,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.37847222222222227</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -635,7 +635,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.38263888888888892</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -649,7 +649,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.38611111111111113</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -663,7 +663,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.3888888888888889</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -677,7 +677,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.39027777777777778</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -691,7 +691,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="1">
-        <v>0.75486111111111109</v>
+        <v>0.3923611111111111</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -705,7 +705,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.39444444444444443</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.3972222222222222</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -733,7 +733,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -747,7 +747,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="1">
-        <v>0.3576388888888889</v>
+        <v>0.40277777777777773</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>